<commit_message>
updated error test template
</commit_message>
<xml_diff>
--- a/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
+++ b/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-publishing-subsidies-service\src\test\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-publishing-subsidies-service\src\test\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B880854-967D-40E4-B2FC-83597525A6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63FD5E3-5144-4E8E-B65D-2463265B3FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -938,13 +938,13 @@
     <t>hggjkfgjfjgjhgjfjgjkdfskjkjbdjkbfjdsbfjdbsfjbdjbfmjhdbmbsmbfjdsbfhbdsjfbdsjhbfjsdbfjdbfjdbfjbdjfbdsjbfkjdsbhsfdbgkjdsbfgjbsdfjgbdsjfhbgjhsddfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgdfgfdgfgfgfgfdgfdgfgfgfgfdgdfgfgfgfgfdggfgfgfgfhgdgdjfsdkjnsvfshjdjcjkkjfjkadjkakjsdjkashiuhadbcbxbkjbckjckjsdkskjbc cmbkjbkjcbsakjckjsckjnsknknscnkjsncknsknknksndksndknaskdnsknsnnssndkjnsdjkhsdskjdnnckjnascknsakjcnkjsanckjnckncknsackjnscknskncknsckncncnnscknsckncncsdsaafddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddddd</t>
   </si>
   <si>
-    <t>a123456b</t>
-  </si>
-  <si>
     <t>500000-1000000</t>
   </si>
   <si>
     <t>BEIS Administrator</t>
+  </si>
+  <si>
+    <t>a123456-</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1548,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1665,7 +1665,7 @@
         <v>186</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>187</v>
@@ -1777,7 +1777,7 @@
         <v>196</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K4" s="21">
         <v>99</v>
@@ -1833,7 +1833,7 @@
         <v>186</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K5" s="21">
         <v>99</v>
@@ -1887,7 +1887,7 @@
         <v>186</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K6" s="21">
         <v>99</v>
@@ -1943,7 +1943,7 @@
         <v>186</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K7" s="21">
         <v>99</v>
@@ -1999,7 +1999,7 @@
         <v>186</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K8" s="21">
         <v>99</v>
@@ -2008,7 +2008,7 @@
         <v>63</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N8" s="24" t="s">
         <v>189</v>
@@ -2057,7 +2057,7 @@
         <v>186</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K9" s="21">
         <v>99</v>
@@ -2108,7 +2108,7 @@
         <v>186</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K10" s="21">
         <v>99</v>
@@ -2159,7 +2159,7 @@
         <v>186</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K11" s="21">
         <v>99</v>
@@ -2177,7 +2177,7 @@
         <v>190</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q11" s="23">
         <v>36210</v>
@@ -14196,8 +14196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A11" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15379,6 +15379,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15746,66 +15796,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
@@ -15841,7 +15832,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15864,23 +15872,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
@@ -15901,6 +15893,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
refactor: reordered excel template columns to reflect front end
</commit_message>
<xml_diff>
--- a/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
+++ b/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-publishing-subsidies-service\src\test\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A32E08B-83BC-47E7-9B61-6CE81D1720E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E8147F-F2B8-4A8B-A6CC-B550436E4878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5652" yWindow="2988" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -1573,7 +1573,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1582,8 +1582,8 @@
     <col min="2" max="2" width="93" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.77734375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="93" style="21" customWidth="1"/>
+    <col min="5" max="5" width="93" style="21" customWidth="1"/>
+    <col min="6" max="7" width="27.77734375" style="21" customWidth="1"/>
     <col min="8" max="8" width="37" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="54.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72.44140625" style="21" bestFit="1" customWidth="1"/>
@@ -1614,14 +1614,14 @@
       <c r="D1" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="35" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>169</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>2</v>
@@ -1680,13 +1680,13 @@
       <c r="D2" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E2" s="24"/>
       <c r="F2" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H2" s="22" t="s">
         <v>80</v>
       </c>
@@ -1744,13 +1744,13 @@
       <c r="D3" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E3" s="24"/>
       <c r="F3" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H3" s="22" t="s">
         <v>193</v>
       </c>
@@ -1804,13 +1804,13 @@
       <c r="D4" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E4" s="24"/>
       <c r="F4" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H4" s="22" t="s">
         <v>193</v>
       </c>
@@ -1866,13 +1866,13 @@
       <c r="D5" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E5" s="24"/>
       <c r="F5" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H5" s="22" t="s">
         <v>193</v>
       </c>
@@ -1926,13 +1926,13 @@
       <c r="D6" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E6" s="24"/>
       <c r="F6" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H6" s="22" t="s">
         <v>193</v>
       </c>
@@ -1988,13 +1988,13 @@
       <c r="D7" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E7" s="24"/>
       <c r="F7" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H7" s="22" t="s">
         <v>193</v>
       </c>
@@ -2050,13 +2050,13 @@
       <c r="D8" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E8" s="24"/>
       <c r="F8" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H8" s="22" t="s">
         <v>193</v>
       </c>
@@ -2114,13 +2114,13 @@
       <c r="D9" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E9" s="24"/>
       <c r="F9" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H9" s="22" t="s">
         <v>193</v>
       </c>
@@ -2171,13 +2171,13 @@
       <c r="D10" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E10" s="24"/>
       <c r="F10" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H10" s="22" t="s">
         <v>193</v>
       </c>
@@ -2228,13 +2228,13 @@
       <c r="D11" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>202</v>
-      </c>
+      <c r="E11" s="24"/>
       <c r="F11" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="24" t="s">
+        <v>202</v>
+      </c>
       <c r="H11" s="22" t="s">
         <v>193</v>
       </c>
@@ -14273,7 +14273,7 @@
           <x14:formula1>
             <xm:f>Dropdown!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D12:F834</xm:sqref>
+          <xm:sqref>D12:D834 F12:G834</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15469,55 +15469,43 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15885,53 +15873,86 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15954,31 +15975,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: Added ability for awards to have multiple subsidy purposes
</commit_message>
<xml_diff>
--- a/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
+++ b/src/test/resource/Bulk_Upload_Awards_Template_local_errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill.batten\Documents\Projects\STS\transparency-db-publishing-subsidies-service\src\test\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-publishing-subsidies-service\src\test\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981DD377-9D94-47D5-8D75-6EB35B73880E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A25C9F-9797-411F-A586-D89A77E585C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -926,9 +926,6 @@
     <t>10.Information and communication</t>
   </si>
   <si>
-    <t>SME support</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
@@ -960,13 +957,16 @@
   </si>
   <si>
     <t>Subsidies or Schemes of Interest (SSoI)</t>
+  </si>
+  <si>
+    <t>Research and development | Training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,6 +1062,12 @@
       <color rgb="FF0B0C0C"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1261,6 +1267,9 @@
     <xf numFmtId="49" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1278,9 +1287,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1585,10 +1591,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1349"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1631,16 +1637,16 @@
         <v>168</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>169</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>200</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>201</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>2</v>
@@ -1702,10 +1708,10 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>80</v>
@@ -1720,7 +1726,7 @@
         <v>186</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>187</v>
@@ -1767,16 +1773,16 @@
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I3" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>25</v>
@@ -1786,7 +1792,7 @@
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O3" s="20" t="s">
         <v>63</v>
@@ -1826,29 +1832,29 @@
         <v>171</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I4" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>80</v>
       </c>
       <c r="L4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>196</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>197</v>
       </c>
       <c r="N4" s="21">
         <v>99</v>
@@ -1893,16 +1899,16 @@
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I5" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>80</v>
@@ -1911,7 +1917,7 @@
         <v>186</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N5" s="21">
         <v>99</v>
@@ -1954,16 +1960,16 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I6" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>18</v>
@@ -1972,7 +1978,7 @@
         <v>186</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N6" s="21">
         <v>99</v>
@@ -2017,16 +2023,16 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I7" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>18</v>
@@ -2035,7 +2041,7 @@
         <v>186</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N7" s="21">
         <v>99</v>
@@ -2080,16 +2086,16 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
       <c r="G8" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I8" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>18</v>
@@ -2098,7 +2104,7 @@
         <v>186</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N8" s="21">
         <v>99</v>
@@ -2107,7 +2113,7 @@
         <v>63</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q8" s="24" t="s">
         <v>189</v>
@@ -2142,21 +2148,21 @@
       <c r="D9" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="42" t="s">
-        <v>204</v>
+      <c r="E9" s="36" t="s">
+        <v>203</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I9" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>18</v>
@@ -2165,7 +2171,7 @@
         <v>186</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N9" s="21">
         <v>99</v>
@@ -2205,16 +2211,16 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I10" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>25</v>
@@ -2223,7 +2229,7 @@
         <v>186</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N10" s="21">
         <v>99</v>
@@ -2260,21 +2266,21 @@
       <c r="D11" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>204</v>
+      <c r="E11" s="36" t="s">
+        <v>203</v>
       </c>
       <c r="F11" s="24"/>
       <c r="G11" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I11" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>194</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>28</v>
@@ -2283,7 +2289,7 @@
         <v>186</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N11" s="21">
         <v>99</v>
@@ -2301,7 +2307,7 @@
         <v>190</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T11" s="23">
         <v>36210</v>
@@ -14248,6 +14254,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -15126,13 +15133,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>113</v>
       </c>
       <c r="D2" s="27" t="s">
@@ -15140,37 +15147,37 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="27" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="27" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>119</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -15178,25 +15185,25 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="13" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="27" t="s">
         <v>117</v>
       </c>
@@ -15293,13 +15300,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>137</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -15307,33 +15314,33 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="13" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="13" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="13" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="27" t="s">
         <v>117</v>
       </c>
@@ -15503,6 +15510,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15870,45 +15906,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -15958,7 +15956,37 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15981,39 +16009,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>